<commit_message>
fix bug export file excel
</commit_message>
<xml_diff>
--- a/DSGV.xlsx
+++ b/DSGV.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t/>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Nguyễn Mạnh Hiếu</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị B</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -104,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:D8"/>
+  <dimension ref="A3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -185,6 +197,48 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
all in export file excel
</commit_message>
<xml_diff>
--- a/DSGV.xlsx
+++ b/DSGV.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t/>
   </si>
   <si>
-    <t>DANH SACH GIA SACH</t>
+    <t>DANH SÁCH GIÁO VIÊN</t>
   </si>
   <si>
     <t>Mã giáo viên</t>
@@ -62,16 +62,31 @@
     <t>Nguyễn Mạnh Hiếu</t>
   </si>
   <si>
-    <t>Nguyễn Thị B</t>
-  </si>
-  <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>NGUYỄN VĂN HÙNG</t>
+  </si>
+  <si>
+    <t>HÀ TÂY</t>
+  </si>
+  <si>
+    <t>031231231</t>
+  </si>
+  <si>
+    <t>HÙNG NGUYỄN VĂN</t>
+  </si>
+  <si>
+    <t>ỨNG HÒA</t>
+  </si>
+  <si>
+    <t>123123123</t>
+  </si>
+  <si>
+    <t>Mạnh hiếu</t>
+  </si>
+  <si>
+    <t>sóc sơn</t>
+  </si>
+  <si>
+    <t>123123</t>
   </si>
 </sst>
 </file>
@@ -205,10 +220,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -216,13 +231,13 @@
         <v>15.0</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -230,13 +245,13 @@
         <v>16.0</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>